<commit_message>
Mod 1 Lab File Charts Design Changed
</commit_message>
<xml_diff>
--- a/Intro to Data Analysis with Excel/1. Intro to reporting in excel/Lab1Start v5.xlsx
+++ b/Intro to Data Analysis with Excel/1. Intro to reporting in excel/Lab1Start v5.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\@jay\Github\Introduction-to-Data-Analysis-with-Excel\Intro to Data Analysis with Excel\1. Intro to reporting in excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -57,7 +62,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -107,7 +112,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -123,26 +128,77 @@
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Yearly</a:t>
+              <a:t>Yearly Category Revenue</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Category Revenue</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.29430666754890933"/>
+          <c:y val="5.0209205020920501E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -164,6 +220,21 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -216,6 +287,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0883-42C3-8E2A-55683392BE88}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -231,6 +307,21 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -289,6 +380,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0883-42C3-8E2A-55683392BE88}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -304,6 +400,21 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -356,6 +467,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0883-42C3-8E2A-55683392BE88}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -371,6 +487,21 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -429,6 +560,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-0883-42C3-8E2A-55683392BE88}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -438,7 +574,6 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="708358144"/>
         <c:axId val="657682944"/>
@@ -451,9 +586,41 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="657682944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -468,25 +635,133 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="708358144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -496,7 +771,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -512,11 +787,27 @@
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
@@ -525,8 +816,48 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10234662635980694"/>
+          <c:y val="6.0882800608828003E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -535,8 +866,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.8099776154419338E-2"/>
-          <c:y val="0.25983359580052495"/>
+          <c:x val="0.22096656006736359"/>
+          <c:y val="0.24771095102473892"/>
           <c:w val="0.48146773871997928"/>
           <c:h val="0.66683307086614174"/>
         </c:manualLayout>
@@ -557,7 +888,161 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -566,6 +1051,24 @@
             <c:showPercent val="1"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="95000"/>
+                      <a:alpha val="54000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -602,6 +1105,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5B47-4CC4-BA88-D6D0E19E9A6D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:dLblPos val="ctr"/>
@@ -615,16 +1123,85 @@
         </c:dLbls>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="1"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -634,7 +1211,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -650,11 +1227,27 @@
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
@@ -665,6 +1258,39 @@
       </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -687,6 +1313,44 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -741,6 +1405,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FD2F-418E-9D26-1FD5C42792D5}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -750,7 +1419,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
         <c:axId val="66146816"/>
         <c:axId val="689034304"/>
       </c:barChart>
@@ -761,9 +1431,42 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="689034304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -778,26 +1481,133 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
-        <c:majorGridlines/>
-        <c:minorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="66146816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="t"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -806,20 +1616,1628 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="257">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -840,16 +3258,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>209549</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -870,16 +3288,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1190,7 +3608,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1200,8 +3618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>